<commit_message>
HOTFIX: fixed LDAP AD authentication, to grant permissions according to AD groups, and to traverse nested AD groups.
Updated target of report links to _blank.
Updated feature registration xlsx to allow more SRIDs.
Recommit, since Apache was still running upon last commit.
</commit_message>
<xml_diff>
--- a/find_artek/static/publications/docs/find-artek_feature_registration.xlsx
+++ b/find_artek/static/publications/docs/find-artek_feature_registration.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="150" windowWidth="15315" windowHeight="12075"/>
@@ -12,7 +12,7 @@
     <sheet name="dd mm ss.ss -&gt; dd.dddd conv" sheetId="3" r:id="rId3"/>
     <sheet name="Example features" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -573,7 +573,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -683,16 +683,61 @@
   <si>
     <t>PHOTO</t>
   </si>
+  <si>
+    <t>WGS 84 / UTM zone 18N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 19N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 20N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 21N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 23N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 24N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 25N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 26N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 27N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 28N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 29N</t>
+  </si>
+  <si>
+    <t>South Greenland (Narsarssuaq, Nanortalik, etc.)</t>
+  </si>
+  <si>
+    <t>East Greenland</t>
+  </si>
+  <si>
+    <t>Upernavik area</t>
+  </si>
+  <si>
+    <t>Thule / Qaanaaq area</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -807,11 +852,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -819,6 +864,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -897,6 +947,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -931,6 +982,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1106,15 +1158,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="11" customWidth="1"/>
@@ -1131,7 +1183,7 @@
     <col min="14" max="20" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" customFormat="1">
+    <row r="1" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -1172,22 +1224,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" customFormat="1">
+    <row r="2" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
       <c r="I2" s="3"/>
       <c r="J2" s="4"/>
       <c r="K2" s="5"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" customFormat="1">
+    <row r="3" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1202,7 +1254,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" customFormat="1">
+    <row r="4" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1217,7 +1269,7 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" customFormat="1">
+    <row r="5" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1232,7 +1284,7 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" customFormat="1">
+    <row r="6" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1247,7 +1299,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" customFormat="1">
+    <row r="7" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1262,7 +1314,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" customFormat="1">
+    <row r="8" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1277,7 +1329,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" customFormat="1">
+    <row r="9" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1292,7 +1344,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" customFormat="1">
+    <row r="10" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1307,7 +1359,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" customFormat="1">
+    <row r="11" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1322,7 +1374,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" customFormat="1">
+    <row r="12" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1337,7 +1389,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" customFormat="1">
+    <row r="13" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1352,7 +1404,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" customFormat="1">
+    <row r="14" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1367,7 +1419,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" customFormat="1">
+    <row r="15" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1382,7 +1434,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" customFormat="1">
+    <row r="16" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1397,7 +1449,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" customFormat="1">
+    <row r="17" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1412,7 +1464,7 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" customFormat="1">
+    <row r="18" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1427,7 +1479,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" customFormat="1">
+    <row r="19" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1442,7 +1494,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" customFormat="1">
+    <row r="20" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1457,7 +1509,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" customFormat="1">
+    <row r="21" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1472,7 +1524,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" customFormat="1">
+    <row r="22" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1487,7 +1539,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" customFormat="1">
+    <row r="23" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1502,7 +1554,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" customFormat="1">
+    <row r="24" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1517,7 +1569,7 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" customFormat="1">
+    <row r="25" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1532,7 +1584,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" customFormat="1">
+    <row r="26" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1547,7 +1599,7 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" customFormat="1">
+    <row r="27" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1562,7 +1614,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" customFormat="1">
+    <row r="28" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1577,7 +1629,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" customFormat="1">
+    <row r="29" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1592,7 +1644,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" customFormat="1">
+    <row r="30" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1607,7 +1659,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" customFormat="1">
+    <row r="31" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1622,7 +1674,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" customFormat="1">
+    <row r="32" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1637,7 +1689,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" customFormat="1">
+    <row r="33" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1652,7 +1704,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" customFormat="1">
+    <row r="34" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1667,7 +1719,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" customFormat="1">
+    <row r="35" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1682,7 +1734,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13" customFormat="1">
+    <row r="36" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1697,7 +1749,7 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" customFormat="1">
+    <row r="37" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1712,7 +1764,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" customFormat="1">
+    <row r="38" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1727,7 +1779,7 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:13" customFormat="1">
+    <row r="39" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1742,7 +1794,7 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" customFormat="1">
+    <row r="40" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1757,7 +1809,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" customFormat="1">
+    <row r="41" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1772,7 +1824,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" customFormat="1">
+    <row r="42" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1787,7 +1839,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" customFormat="1">
+    <row r="43" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1802,7 +1854,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" customFormat="1">
+    <row r="44" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1817,7 +1869,7 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13" customFormat="1">
+    <row r="45" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1832,7 +1884,7 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" customFormat="1">
+    <row r="46" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1847,7 +1899,7 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13" customFormat="1">
+    <row r="47" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1862,7 +1914,7 @@
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" customFormat="1">
+    <row r="48" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1877,7 +1929,7 @@
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" customFormat="1">
+    <row r="49" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1892,7 +1944,7 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" customFormat="1">
+    <row r="50" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1907,7 +1959,7 @@
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13" customFormat="1">
+    <row r="51" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -1922,7 +1974,7 @@
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" customFormat="1">
+    <row r="52" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1937,7 +1989,7 @@
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13" customFormat="1">
+    <row r="53" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1952,7 +2004,7 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" customFormat="1">
+    <row r="54" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -1967,7 +2019,7 @@
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13" customFormat="1">
+    <row r="55" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -1982,7 +2034,7 @@
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
     </row>
-    <row r="56" spans="1:13" customFormat="1">
+    <row r="56" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -1997,7 +2049,7 @@
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
     </row>
-    <row r="57" spans="1:13" customFormat="1">
+    <row r="57" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -2012,7 +2064,7 @@
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="1:13" customFormat="1">
+    <row r="58" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -2027,7 +2079,7 @@
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="1:13" customFormat="1">
+    <row r="59" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -2042,7 +2094,7 @@
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
     </row>
-    <row r="60" spans="1:13" customFormat="1">
+    <row r="60" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -2057,7 +2109,7 @@
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
     </row>
-    <row r="61" spans="1:13" customFormat="1">
+    <row r="61" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -2072,7 +2124,7 @@
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" spans="1:13" customFormat="1">
+    <row r="62" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -2087,7 +2139,7 @@
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
     </row>
-    <row r="63" spans="1:13" customFormat="1">
+    <row r="63" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -2102,7 +2154,7 @@
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
     </row>
-    <row r="64" spans="1:13" customFormat="1">
+    <row r="64" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -2117,7 +2169,7 @@
       <c r="L64" s="3"/>
       <c r="M64" s="3"/>
     </row>
-    <row r="65" spans="1:20">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -2139,7 +2191,7 @@
       <c r="S65"/>
       <c r="T65"/>
     </row>
-    <row r="66" spans="1:20">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -2161,7 +2213,7 @@
       <c r="S66"/>
       <c r="T66"/>
     </row>
-    <row r="67" spans="1:20">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -2183,7 +2235,7 @@
       <c r="S67"/>
       <c r="T67"/>
     </row>
-    <row r="68" spans="1:20">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -2205,7 +2257,7 @@
       <c r="S68"/>
       <c r="T68"/>
     </row>
-    <row r="69" spans="1:20">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -2227,7 +2279,7 @@
       <c r="S69"/>
       <c r="T69"/>
     </row>
-    <row r="70" spans="1:20">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -2249,7 +2301,7 @@
       <c r="S70"/>
       <c r="T70"/>
     </row>
-    <row r="71" spans="1:20">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -2271,7 +2323,7 @@
       <c r="S71"/>
       <c r="T71"/>
     </row>
-    <row r="72" spans="1:20">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -2293,7 +2345,7 @@
       <c r="S72"/>
       <c r="T72"/>
     </row>
-    <row r="73" spans="1:20">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -2315,7 +2367,7 @@
       <c r="S73"/>
       <c r="T73"/>
     </row>
-    <row r="74" spans="1:20">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -2337,7 +2389,7 @@
       <c r="S74"/>
       <c r="T74"/>
     </row>
-    <row r="75" spans="1:20">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -2359,7 +2411,7 @@
       <c r="S75"/>
       <c r="T75"/>
     </row>
-    <row r="76" spans="1:20">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -2381,7 +2433,7 @@
       <c r="S76"/>
       <c r="T76"/>
     </row>
-    <row r="77" spans="1:20">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -2403,7 +2455,7 @@
       <c r="S77"/>
       <c r="T77"/>
     </row>
-    <row r="78" spans="1:20">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -2427,7 +2479,7 @@
     </row>
   </sheetData>
   <sheetProtection password="CC3D" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0" sort="0"/>
-  <dataValidations count="5">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
       <formula1>"point"</formula1>
     </dataValidation>
@@ -2437,9 +2489,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="The field value must be taken from the list of choices." sqref="I2:I1048576">
       <formula1>"Approximate, GPS (phase), GPS (code), Unknown"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="F2:F1048576">
-      <formula1>"3182,4326,32622"</formula1>
-    </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
       <formula1>COUNTIF($B:$B,B1)&lt;2</formula1>
     </dataValidation>
@@ -2447,25 +2496,37 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>'SRID list'!$B$2:$B$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A23" sqref="A23:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
     <col min="4" max="4" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>21</v>
       </c>
@@ -2479,7 +2540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2493,7 +2554,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2507,156 +2568,246 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1">
+        <v>32618</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>32619</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>32620</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>32621</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
         <v>32622</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>32623</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>32624</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>32625</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>32626</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>32627</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>32628</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>32629</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1"/>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="24" spans="1:4" ht="126.75" customHeight="1">
-      <c r="A24" s="17" t="s">
+    <row r="23" spans="1:4" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
     </row>
   </sheetData>
   <sortState ref="A2:D24">
     <sortCondition ref="B2:B24"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="4.140625" customWidth="1"/>
     <col min="8" max="8" width="4.140625" customWidth="1"/>
@@ -2665,7 +2816,7 @@
     <col min="11" max="12" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2687,7 +2838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -2717,7 +2868,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2748,7 +2899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I4" s="8" t="s">
         <v>18</v>
       </c>
@@ -2761,7 +2912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I5" s="8" t="s">
         <v>18</v>
       </c>
@@ -2774,7 +2925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I6" s="8" t="s">
         <v>18</v>
       </c>
@@ -2787,7 +2938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I7" s="8" t="s">
         <v>18</v>
       </c>
@@ -2800,7 +2951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I8" s="8" t="s">
         <v>18</v>
       </c>
@@ -2813,7 +2964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I9" s="8" t="s">
         <v>18</v>
       </c>
@@ -2826,7 +2977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I10" s="8" t="s">
         <v>18</v>
       </c>
@@ -2839,7 +2990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I11" s="8" t="s">
         <v>18</v>
       </c>
@@ -2852,7 +3003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I12" s="8" t="s">
         <v>18</v>
       </c>
@@ -2865,7 +3016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I13" s="8" t="s">
         <v>18</v>
       </c>
@@ -2878,7 +3029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I14" s="8" t="s">
         <v>18</v>
       </c>
@@ -2891,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I15" s="8" t="s">
         <v>18</v>
       </c>
@@ -2904,7 +3055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I16" s="8" t="s">
         <v>18</v>
       </c>
@@ -2917,7 +3068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="9:12">
+    <row r="17" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I17" s="8" t="s">
         <v>18</v>
       </c>
@@ -2930,7 +3081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="9:12">
+    <row r="18" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I18" s="8" t="s">
         <v>18</v>
       </c>
@@ -2943,7 +3094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="9:12">
+    <row r="19" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I19" s="8" t="s">
         <v>18</v>
       </c>
@@ -2956,7 +3107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="9:12">
+    <row r="20" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I20" s="8" t="s">
         <v>18</v>
       </c>
@@ -2969,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="9:12">
+    <row r="21" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I21" s="8" t="s">
         <v>18</v>
       </c>
@@ -2982,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="9:12">
+    <row r="22" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I22" s="8" t="s">
         <v>18</v>
       </c>
@@ -2995,7 +3146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="9:12">
+    <row r="23" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I23" s="8" t="s">
         <v>18</v>
       </c>
@@ -3014,14 +3165,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
@@ -3038,7 +3189,7 @@
     <col min="13" max="13" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -3079,7 +3230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>375</v>
       </c>
@@ -3098,10 +3249,10 @@
       <c r="F2" s="3">
         <v>32622</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="17">
         <v>382585.55</v>
       </c>
-      <c r="H2" s="18">
+      <c r="H2" s="17">
         <v>7427269.1699999999</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -3116,7 +3267,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>375</v>
       </c>
@@ -3153,7 +3304,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>

</xml_diff>

<commit_message>
Template for uploading features updated to allow lines and polygons. sheets protected with password 1234.
</commit_message>
<xml_diff>
--- a/find_artek/static/publications/docs/find-artek_feature_registration.xlsx
+++ b/find_artek/static/publications/docs/find-artek_feature_registration.xlsx
@@ -10,7 +10,8 @@
     <sheet name="Features" sheetId="1" r:id="rId1"/>
     <sheet name="SRID list" sheetId="2" r:id="rId2"/>
     <sheet name="dd mm ss.ss -&gt; dd.dddd conv" sheetId="3" r:id="rId3"/>
-    <sheet name="Example features" sheetId="4" r:id="rId4"/>
+    <sheet name="Example features" sheetId="5" r:id="rId4"/>
+    <sheet name="UTM zone map" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -66,7 +67,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Feature identifier used to determine if geometries are to be added to the same or a new feature object. One feature may consist of several points f.ex. - in which case the Feature#-column should hold the same value for all geometries. Non-geometry fields (e.g. name, description etc. is read from the first row reffering to a specific feature#.</t>
+Feature identifier used to determine if geometries are to be added to the same or a new feature object. A line feature, f.ex. consists of several points - in which case the Feature#-column should hold the same value for all the rows that are to be added to the same line feature. The rows will be added to the line/polygon in the order they occur in the sheet. The feature type and srid must be the same in all rows that are to be added to the same line/polygon. 
+Non-geometry fields (e.g. name, description etc.) is read from the first row reffering to a specific feature#.</t>
         </r>
       </text>
     </comment>
@@ -114,7 +116,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Choose from drop down list (only geometry type "point" supported.</t>
+Choose from drop down list (point, line or polygon)</t>
         </r>
       </text>
     </comment>
@@ -138,7 +140,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Choose as appropriate from drop down list</t>
+Choose the appropriate spatial reference id (srid) from the drop down list.
+The srid depends on how the coordinates were obtained and processed.</t>
         </r>
       </text>
     </comment>
@@ -252,7 +255,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Thomas Ingeman-Nielsen:</t>
+          <t xml:space="preserve">Thomas Ingeman-Nielsen:
+</t>
         </r>
         <r>
           <rPr>
@@ -261,7 +265,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
+          <t>A meaningful textual description of the feature. Could include information on what measurements or observations were obtained, main results, etc.
 Use ALT+ENTER to make a line break inside a cell.</t>
         </r>
       </text>
@@ -286,7 +290,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Mainly used for images, the direction in which the image was taken.</t>
+Mainly used for images: the cardinal direction (N, S, E, W, SE, NW, etc.) in which the image was taken.</t>
         </r>
       </text>
     </comment>
@@ -344,7 +348,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Feature identifier used to determine if geometries are to be added to the same or a new feature object. One feature may consist of several points f.ex. - in which case the Feature#-column should hold the same value for all geometries. Non-geometry fields (e.g. name, description etc. is read from the first row reffering to a specific feature#.</t>
+Feature identifier used to determine if geometries are to be added to the same or a new feature object. A line feature, f.ex. consists of several points - in which case the Feature#-column should hold the same value for all the rows that are to be added to the same line feature. The rows will be added to the line/polygon in the order they occur in the sheet. The feature type and srid must be the same in all rows that are to be added to the same line/polygon. 
+Non-geometry fields (e.g. name, description etc.) is read from the first row reffering to a specific feature#.</t>
         </r>
       </text>
     </comment>
@@ -392,7 +397,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Choose from drop down list (only geometry type "point" supported.</t>
+Choose from drop down list (point, line or polygon)</t>
         </r>
       </text>
     </comment>
@@ -416,7 +421,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Choose as appropriate from drop down list</t>
+Choose the appropriate spatial reference id (srid) from the drop down list.
+The srid depends on how the coordinates were obtained and processed.</t>
         </r>
       </text>
     </comment>
@@ -530,7 +536,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Thomas Ingeman-Nielsen:</t>
+          <t xml:space="preserve">Thomas Ingeman-Nielsen:
+</t>
         </r>
         <r>
           <rPr>
@@ -539,7 +546,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
+          <t>A meaningful textual description of the feature. Could include information on what measurements or observations were obtained, main results, etc.
 Use ALT+ENTER to make a line break inside a cell.</t>
         </r>
       </text>
@@ -564,7 +571,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Mainly used for images, the direction in which the image was taken.</t>
+Mainly used for images: the cardinal direction (N, S, E, W, SE, NW, etc.) in which the image was taken.</t>
         </r>
       </text>
     </comment>
@@ -573,7 +580,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -608,9 +615,6 @@
     <t>Geometry_type</t>
   </si>
   <si>
-    <t>WGS84 Lon/Lat</t>
-  </si>
-  <si>
     <t>WGS 84 / UTM zone 22N</t>
   </si>
   <si>
@@ -644,89 +648,180 @@
     <t>SRID code</t>
   </si>
   <si>
-    <t>Global projection</t>
-  </si>
-  <si>
     <t>Most of West Greenland covered</t>
   </si>
   <si>
     <t>GR96 / UTM zone 22N</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>GEUS hus 1</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
+    <t>Approximate</t>
+  </si>
+  <si>
+    <t>Testing Import feature from file - UTM coords</t>
+  </si>
+  <si>
+    <t>Testing Import feature from file - LON/LAT coords</t>
+  </si>
+  <si>
+    <t>GEUS hus 2</t>
+  </si>
+  <si>
+    <t>PHOTO</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 18N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 19N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 20N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 21N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 23N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 24N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 25N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 26N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 27N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 28N</t>
+  </si>
+  <si>
+    <t>WGS 84 / UTM zone 29N</t>
+  </si>
+  <si>
+    <t>South Greenland (Narsarssuaq, Nanortalik, etc.)</t>
+  </si>
+  <si>
+    <t>East Greenland</t>
+  </si>
+  <si>
+    <t>Upernavik area</t>
+  </si>
+  <si>
+    <t>Thule / Qaanaaq area</t>
+  </si>
+  <si>
+    <t>WGS84 Longitude/Latitude</t>
+  </si>
+  <si>
+    <t>Global system, geographical coordinates</t>
+  </si>
+  <si>
+    <t>BOREHOLE</t>
+  </si>
+  <si>
+    <t>txt_code</t>
+  </si>
+  <si>
+    <t>utm22_gr96</t>
+  </si>
+  <si>
+    <t>geo_wgs84</t>
+  </si>
+  <si>
+    <t>utm18_wgs84</t>
+  </si>
+  <si>
+    <t>utm19_wgs84</t>
+  </si>
+  <si>
+    <t>utm20_wgs84</t>
+  </si>
+  <si>
+    <t>utm21_wgs84</t>
+  </si>
+  <si>
+    <t>utm22_wgs84</t>
+  </si>
+  <si>
+    <t>utm23_wgs84</t>
+  </si>
+  <si>
+    <t>utm24_wgs84</t>
+  </si>
+  <si>
+    <t>utm25_wgs84</t>
+  </si>
+  <si>
+    <t>utm26_wgs84</t>
+  </si>
+  <si>
+    <t>utm27_wgs84</t>
+  </si>
+  <si>
+    <t>utm28_wgs84</t>
+  </si>
+  <si>
+    <t>utm29_wgs84</t>
+  </si>
+  <si>
+    <t>GPS (phase)</t>
+  </si>
+  <si>
+    <t>Boring BG01, 11821 Forundersøgelser E2013</t>
+  </si>
+  <si>
+    <t>ERT line LG, 11821 Forundersøgelser E2013</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>ERT LG</t>
+  </si>
+  <si>
+    <t>GEOPHYSICAL DATA</t>
+  </si>
+  <si>
+    <t>Borehole BG01</t>
+  </si>
+  <si>
+    <t>Boring BL01, 11821 Forundersøgelser E2013</t>
+  </si>
+  <si>
+    <t>Borehole BL01</t>
+  </si>
+  <si>
+    <t>Area LG</t>
+  </si>
+  <si>
+    <t>polygon</t>
+  </si>
+  <si>
+    <t>Test polygon area import</t>
+  </si>
+  <si>
+    <t>Source: http://www.dmap.co.uk/utmworld.htm</t>
   </si>
   <si>
     <t>These are the most commonly used Spatial Reference IDs  used for coordinates in Greenland.
 Any standard SRID code is understood by the database. A more complete list of SRID codes can be found at:
 http://www.epsg-registry.org/
 Read more about SRIDs at:
-http://www.gaia-gis.it/gaia-sins/spatialite-cookbook/html/srid.html</t>
-  </si>
-  <si>
-    <t>point</t>
-  </si>
-  <si>
-    <t>GEUS hus 1</t>
-  </si>
-  <si>
-    <t>OTHER</t>
-  </si>
-  <si>
-    <t>Approximate</t>
-  </si>
-  <si>
-    <t>Testing Import feature from file - UTM coords</t>
-  </si>
-  <si>
-    <t>Testing Import feature from file - LON/LAT coords</t>
-  </si>
-  <si>
-    <t>GEUS hus 2</t>
-  </si>
-  <si>
-    <t>PHOTO</t>
-  </si>
-  <si>
-    <t>WGS 84 / UTM zone 18N</t>
-  </si>
-  <si>
-    <t>WGS 84 / UTM zone 19N</t>
-  </si>
-  <si>
-    <t>WGS 84 / UTM zone 20N</t>
-  </si>
-  <si>
-    <t>WGS 84 / UTM zone 21N</t>
-  </si>
-  <si>
-    <t>WGS 84 / UTM zone 23N</t>
-  </si>
-  <si>
-    <t>WGS 84 / UTM zone 24N</t>
-  </si>
-  <si>
-    <t>WGS 84 / UTM zone 25N</t>
-  </si>
-  <si>
-    <t>WGS 84 / UTM zone 26N</t>
-  </si>
-  <si>
-    <t>WGS 84 / UTM zone 27N</t>
-  </si>
-  <si>
-    <t>WGS 84 / UTM zone 28N</t>
-  </si>
-  <si>
-    <t>WGS 84 / UTM zone 29N</t>
-  </si>
-  <si>
-    <t>South Greenland (Narsarssuaq, Nanortalik, etc.)</t>
-  </si>
-  <si>
-    <t>East Greenland</t>
-  </si>
-  <si>
-    <t>Upernavik area</t>
-  </si>
-  <si>
-    <t>Thule / Qaanaaq area</t>
+http://www.gaia-gis.it/gaia-sins/spatialite-cookbook/html/srid.html
+A UTM zone map can be found in the sheet named "UTM zone map"</t>
   </si>
 </sst>
 </file>
@@ -808,7 +903,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -855,6 +950,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -870,6 +966,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="http://www.dmap.co.uk/utmworld.gif"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="15935325" cy="8143875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1163,7 +1319,7 @@
   <dimension ref="A1:T78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,7 +1329,7 @@
     <col min="3" max="3" width="15.7109375" style="11" customWidth="1"/>
     <col min="4" max="4" width="23.140625" style="11" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" style="11" customWidth="1"/>
+    <col min="6" max="6" width="14" style="11" customWidth="1"/>
     <col min="7" max="8" width="15.85546875" style="11" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" style="11" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" style="12" customWidth="1"/>
@@ -1185,7 +1341,7 @@
   <sheetData>
     <row r="1" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
@@ -1209,7 +1365,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1</v>
@@ -1291,8 +1447,8 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
       <c r="I6" s="3"/>
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
@@ -2480,16 +2636,16 @@
   </sheetData>
   <sheetProtection password="CC3D" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0" sort="0"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
-      <formula1>"point"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>"GEOPHYSICAL DATA,FIELD MEASUREMENT,RESOURCE,PHOTO,SAMPLE,OTHER,BOREHOLE,LAB MEASUREMENT"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="The field value must be taken from the list of choices." sqref="I2:I1048576">
       <formula1>"Approximate, GPS (phase), GPS (code), Unknown"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+      <formula1>"point,line,polygon"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
       <formula1>COUNTIF($B:$B,B1)&lt;2</formula1>
     </dataValidation>
   </dataValidations>
@@ -2513,62 +2669,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D23"/>
+      <selection activeCell="A23" sqref="A23:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18">
+        <v>3182</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>3182</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="18">
         <v>4326</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2576,25 +2742,31 @@
         <v>32618</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+        <v>53</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="18">
         <v>32619</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2602,53 +2774,65 @@
         <v>32620</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+        <v>55</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="18">
         <v>32621</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="C7" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="18">
         <v>32622</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="C8" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="18">
         <v>32623</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2656,13 +2840,16 @@
         <v>32624</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2670,13 +2857,16 @@
         <v>32625</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2684,13 +2874,16 @@
         <v>32626</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2698,13 +2891,16 @@
         <v>32627</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2712,13 +2908,16 @@
         <v>32628</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2726,74 +2925,85 @@
         <v>32629</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-    </row>
-    <row r="23" spans="1:4" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="23" spans="1:5" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
     </row>
   </sheetData>
+  <sheetProtection password="CC3D" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0" sort="0"/>
   <sortState ref="A2:D24">
     <sortCondition ref="B2:B24"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A23:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2804,7 +3014,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,13 +3028,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="2"/>
       <c r="E1" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -2832,89 +3042,71 @@
       <c r="I1" s="7"/>
       <c r="J1" s="2"/>
       <c r="K1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>16</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="7"/>
       <c r="J2" s="2"/>
       <c r="K2" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="I3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="10">
+        <f>IF(A3&gt;=0,A3+B3/60+C3/3600,A3-B3/60-C3/3600)</f>
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="10">
-        <f>A3+B3/60+C3/3600</f>
-        <v>0</v>
-      </c>
       <c r="L3" s="10">
-        <f>E3+F3/60+G3/3600</f>
+        <f>IF(E3&gt;=0,E3+F3/60+G3/3600,E3-F3/60-G3/3600)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I4" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" s="10">
-        <f t="shared" ref="K4:K23" si="0">A4+B4/60+C4/3600</f>
+        <f t="shared" ref="K4:K23" si="0">IF(A4&gt;=0,A4+B4/60+C4/3600,A4-B4/60-C4/3600)</f>
         <v>0</v>
       </c>
       <c r="L4" s="10">
-        <f t="shared" ref="L4:L23" si="1">E4+F4/60+G4/3600</f>
+        <f t="shared" ref="L4:L23" si="1">IF(E4&gt;=0,E4+F4/60+G4/3600,E4-F4/60-G4/3600)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I5" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" si="0"/>
@@ -2927,7 +3119,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" s="10">
         <f t="shared" si="0"/>
@@ -2940,7 +3132,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I7" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K7" s="10">
         <f t="shared" si="0"/>
@@ -2953,7 +3145,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I8" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K8" s="10">
         <f t="shared" si="0"/>
@@ -2966,7 +3158,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I9" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9" s="10">
         <f t="shared" si="0"/>
@@ -2979,7 +3171,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I10" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K10" s="10">
         <f t="shared" si="0"/>
@@ -2992,7 +3184,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I11" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K11" s="10">
         <f t="shared" si="0"/>
@@ -3005,7 +3197,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I12" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K12" s="10">
         <f t="shared" si="0"/>
@@ -3018,7 +3210,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I13" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K13" s="10">
         <f t="shared" si="0"/>
@@ -3031,7 +3223,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I14" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K14" s="10">
         <f t="shared" si="0"/>
@@ -3044,7 +3236,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I15" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K15" s="10">
         <f t="shared" si="0"/>
@@ -3057,7 +3249,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I16" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K16" s="10">
         <f t="shared" si="0"/>
@@ -3070,7 +3262,7 @@
     </row>
     <row r="17" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I17" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K17" s="10">
         <f t="shared" si="0"/>
@@ -3083,7 +3275,7 @@
     </row>
     <row r="18" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I18" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K18" s="10">
         <f t="shared" si="0"/>
@@ -3096,7 +3288,7 @@
     </row>
     <row r="19" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I19" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K19" s="10">
         <f t="shared" si="0"/>
@@ -3109,7 +3301,7 @@
     </row>
     <row r="20" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I20" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K20" s="10">
         <f t="shared" si="0"/>
@@ -3122,7 +3314,7 @@
     </row>
     <row r="21" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I21" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K21" s="10">
         <f t="shared" si="0"/>
@@ -3135,7 +3327,7 @@
     </row>
     <row r="22" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I22" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K22" s="10">
         <f t="shared" si="0"/>
@@ -3148,7 +3340,7 @@
     </row>
     <row r="23" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I23" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K23" s="10">
         <f t="shared" si="0"/>
@@ -3166,32 +3358,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:T78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="11" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="11" customWidth="1"/>
+    <col min="7" max="8" width="15.85546875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="12" customWidth="1"/>
+    <col min="11" max="11" width="60" style="13" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" style="11" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="11" customWidth="1"/>
+    <col min="14" max="20" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
@@ -3215,7 +3407,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1</v>
@@ -3229,8 +3421,15 @@
       <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+      <c r="S1"/>
+      <c r="T1"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>375</v>
       </c>
@@ -3238,13 +3437,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3">
         <v>32622</v>
@@ -3256,18 +3455,25 @@
         <v>7427269.1699999999</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J2" s="4">
         <v>41336</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>375</v>
       </c>
@@ -3275,13 +3481,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F3" s="3">
         <v>4326</v>
@@ -3293,51 +3499,1875 @@
         <v>66.940393869999994</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J3" s="4">
         <v>41336</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="5"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>413</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3182</v>
+      </c>
+      <c r="G4" s="17">
+        <v>384068.67800000001</v>
+      </c>
+      <c r="H4" s="17">
+        <v>7427054.409</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="4">
+        <v>41541</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>413</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3182</v>
+      </c>
+      <c r="G5" s="17">
+        <v>384138.38</v>
+      </c>
+      <c r="H5" s="17">
+        <v>7427077.1600000001</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="4">
+        <v>41541</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>413</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3182</v>
+      </c>
+      <c r="G6" s="3">
+        <v>384083.82799999998</v>
+      </c>
+      <c r="H6" s="3">
+        <v>7427054.3329999996</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J6" s="4">
+        <v>41541</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>413</v>
+      </c>
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3182</v>
+      </c>
+      <c r="G7" s="3">
+        <v>384054.201</v>
+      </c>
+      <c r="H7" s="3">
+        <v>7427055.0159999998</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>413</v>
+      </c>
+      <c r="B8" s="3">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3182</v>
+      </c>
+      <c r="G8" s="3">
+        <v>384024.27299999999</v>
+      </c>
+      <c r="H8" s="3">
+        <v>7427056.0039999997</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>413</v>
+      </c>
+      <c r="B9" s="3">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3182</v>
+      </c>
+      <c r="G9" s="3">
+        <v>384083.82799999998</v>
+      </c>
+      <c r="H9" s="3">
+        <v>7427254.3329999996</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="4">
+        <v>41541</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>413</v>
+      </c>
+      <c r="B10" s="3">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3182</v>
+      </c>
+      <c r="G10" s="3">
+        <v>384054.201</v>
+      </c>
+      <c r="H10" s="3">
+        <v>7427155.0159999998</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>413</v>
+      </c>
+      <c r="B11" s="3">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="3">
+        <v>3182</v>
+      </c>
+      <c r="G11" s="3">
+        <v>384024.27299999999</v>
+      </c>
+      <c r="H11" s="3">
+        <v>7427256.0039999997</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+      <c r="R29"/>
+      <c r="S29"/>
+      <c r="T29"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42"/>
+      <c r="O42"/>
+      <c r="P42"/>
+      <c r="Q42"/>
+      <c r="R42"/>
+      <c r="S42"/>
+      <c r="T42"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43"/>
+      <c r="O43"/>
+      <c r="P43"/>
+      <c r="Q43"/>
+      <c r="R43"/>
+      <c r="S43"/>
+      <c r="T43"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+      <c r="R44"/>
+      <c r="S44"/>
+      <c r="T44"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47"/>
+      <c r="O47"/>
+      <c r="P47"/>
+      <c r="Q47"/>
+      <c r="R47"/>
+      <c r="S47"/>
+      <c r="T47"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48"/>
+      <c r="O48"/>
+      <c r="P48"/>
+      <c r="Q48"/>
+      <c r="R48"/>
+      <c r="S48"/>
+      <c r="T48"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49"/>
+      <c r="O49"/>
+      <c r="P49"/>
+      <c r="Q49"/>
+      <c r="R49"/>
+      <c r="S49"/>
+      <c r="T49"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50"/>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+      <c r="R50"/>
+      <c r="S50"/>
+      <c r="T50"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51"/>
+      <c r="O51"/>
+      <c r="P51"/>
+      <c r="Q51"/>
+      <c r="R51"/>
+      <c r="S51"/>
+      <c r="T51"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52"/>
+      <c r="O52"/>
+      <c r="P52"/>
+      <c r="Q52"/>
+      <c r="R52"/>
+      <c r="S52"/>
+      <c r="T52"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53"/>
+      <c r="O53"/>
+      <c r="P53"/>
+      <c r="Q53"/>
+      <c r="R53"/>
+      <c r="S53"/>
+      <c r="T53"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54"/>
+      <c r="O54"/>
+      <c r="P54"/>
+      <c r="Q54"/>
+      <c r="R54"/>
+      <c r="S54"/>
+      <c r="T54"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55"/>
+      <c r="O55"/>
+      <c r="P55"/>
+      <c r="Q55"/>
+      <c r="R55"/>
+      <c r="S55"/>
+      <c r="T55"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56"/>
+      <c r="O56"/>
+      <c r="P56"/>
+      <c r="Q56"/>
+      <c r="R56"/>
+      <c r="S56"/>
+      <c r="T56"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57"/>
+      <c r="O57"/>
+      <c r="P57"/>
+      <c r="Q57"/>
+      <c r="R57"/>
+      <c r="S57"/>
+      <c r="T57"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58"/>
+      <c r="O58"/>
+      <c r="P58"/>
+      <c r="Q58"/>
+      <c r="R58"/>
+      <c r="S58"/>
+      <c r="T58"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59"/>
+      <c r="O59"/>
+      <c r="P59"/>
+      <c r="Q59"/>
+      <c r="R59"/>
+      <c r="S59"/>
+      <c r="T59"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60"/>
+      <c r="O60"/>
+      <c r="P60"/>
+      <c r="Q60"/>
+      <c r="R60"/>
+      <c r="S60"/>
+      <c r="T60"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61"/>
+      <c r="O61"/>
+      <c r="P61"/>
+      <c r="Q61"/>
+      <c r="R61"/>
+      <c r="S61"/>
+      <c r="T61"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62"/>
+      <c r="O62"/>
+      <c r="P62"/>
+      <c r="Q62"/>
+      <c r="R62"/>
+      <c r="S62"/>
+      <c r="T62"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63"/>
+      <c r="O63"/>
+      <c r="P63"/>
+      <c r="Q63"/>
+      <c r="R63"/>
+      <c r="S63"/>
+      <c r="T63"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="3"/>
+      <c r="N64"/>
+      <c r="O64"/>
+      <c r="P64"/>
+      <c r="Q64"/>
+      <c r="R64"/>
+      <c r="S64"/>
+      <c r="T64"/>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65"/>
+      <c r="O65"/>
+      <c r="P65"/>
+      <c r="Q65"/>
+      <c r="R65"/>
+      <c r="S65"/>
+      <c r="T65"/>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
+      <c r="N66"/>
+      <c r="O66"/>
+      <c r="P66"/>
+      <c r="Q66"/>
+      <c r="R66"/>
+      <c r="S66"/>
+      <c r="T66"/>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67"/>
+      <c r="O67"/>
+      <c r="P67"/>
+      <c r="Q67"/>
+      <c r="R67"/>
+      <c r="S67"/>
+      <c r="T67"/>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68"/>
+      <c r="O68"/>
+      <c r="P68"/>
+      <c r="Q68"/>
+      <c r="R68"/>
+      <c r="S68"/>
+      <c r="T68"/>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3"/>
+      <c r="N69"/>
+      <c r="O69"/>
+      <c r="P69"/>
+      <c r="Q69"/>
+      <c r="R69"/>
+      <c r="S69"/>
+      <c r="T69"/>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
+      <c r="N70"/>
+      <c r="O70"/>
+      <c r="P70"/>
+      <c r="Q70"/>
+      <c r="R70"/>
+      <c r="S70"/>
+      <c r="T70"/>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3"/>
+      <c r="N71"/>
+      <c r="O71"/>
+      <c r="P71"/>
+      <c r="Q71"/>
+      <c r="R71"/>
+      <c r="S71"/>
+      <c r="T71"/>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="5"/>
+      <c r="L72" s="3"/>
+      <c r="M72" s="3"/>
+      <c r="N72"/>
+      <c r="O72"/>
+      <c r="P72"/>
+      <c r="Q72"/>
+      <c r="R72"/>
+      <c r="S72"/>
+      <c r="T72"/>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="5"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+      <c r="N73"/>
+      <c r="O73"/>
+      <c r="P73"/>
+      <c r="Q73"/>
+      <c r="R73"/>
+      <c r="S73"/>
+      <c r="T73"/>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="5"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="3"/>
+      <c r="N74"/>
+      <c r="O74"/>
+      <c r="P74"/>
+      <c r="Q74"/>
+      <c r="R74"/>
+      <c r="S74"/>
+      <c r="T74"/>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75"/>
+      <c r="O75"/>
+      <c r="P75"/>
+      <c r="Q75"/>
+      <c r="R75"/>
+      <c r="S75"/>
+      <c r="T75"/>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
+      <c r="N76"/>
+      <c r="O76"/>
+      <c r="P76"/>
+      <c r="Q76"/>
+      <c r="R76"/>
+      <c r="S76"/>
+      <c r="T76"/>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="5"/>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77"/>
+      <c r="O77"/>
+      <c r="P77"/>
+      <c r="Q77"/>
+      <c r="R77"/>
+      <c r="S77"/>
+      <c r="T77"/>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="5"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3"/>
+      <c r="N78"/>
+      <c r="O78"/>
+      <c r="P78"/>
+      <c r="Q78"/>
+      <c r="R78"/>
+      <c r="S78"/>
+      <c r="T78"/>
     </row>
   </sheetData>
-  <dataValidations count="5">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B4">
-      <formula1>COUNTIF($B:$B,B1)&lt;2</formula1>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0" sort="0"/>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E1048576 E4:E8 E9:E11">
+      <formula1>"point,line,polygon"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="F2:F4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3">
+      <formula1>"point"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="F2:F3">
       <formula1>"3182,4326,32622"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="The field value must be taken from the list of choices." sqref="I2:I4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="The field value must be taken from the list of choices." sqref="I12:I1048576 I2:I8 I9:I11">
       <formula1>"Approximate, GPS (phase), GPS (code), Unknown"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C1048576 C2:C8 C9:C11">
       <formula1>"GEOPHYSICAL DATA,FIELD MEASUREMENT,RESOURCE,PHOTO,SAMPLE,OTHER,BOREHOLE,LAB MEASUREMENT"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4">
-      <formula1>"point"</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B3">
+      <formula1>COUNTIF($B:$B,B1)&lt;2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>'SRID list'!$B$2:$B$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>F12:F1048576 F4:F8 F9:F11</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FIXED: xlsx template for features now allows lines and polys, and the transformation from dd mm ss to dd.dddd has been corrected.
</commit_message>
<xml_diff>
--- a/find_artek/static/publications/docs/find-artek_feature_registration.xlsx
+++ b/find_artek/static/publications/docs/find-artek_feature_registration.xlsx
@@ -66,7 +66,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Feature identifier used to determine if geometries are to be added to the same or a new feature object. One feature may consist of several points f.ex. - in which case the Feature#-column should hold the same value for all geometries. Non-geometry fields (e.g. name, description etc. is read from the first row reffering to a specific feature#.</t>
+Feature identifier used to determine if geometries are to be added to the same or a new feature object. A line feature, f.ex. consists of several points - in which case the Feature#-column should hold the same value for all the rows that are to be added to the same line feature. The rows will be added to the line/polygon in the order they occur in the sheet. The feature type and srid must be the same in all rows that are to be added to the same line/polygon. 
+Non-geometry fields (e.g. name, description etc.) is read from the first row reffering to a specific feature#.</t>
         </r>
       </text>
     </comment>
@@ -114,7 +115,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Choose from drop down list (only geometry type "point" supported.</t>
+Choose from drop down list (point, line or polygon)</t>
         </r>
       </text>
     </comment>
@@ -138,7 +139,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Choose as appropriate from drop down list</t>
+Choose the appropriate spatial reference id (srid) from the drop down list.
+The srid depends on how the coordinates were obtained and processed.</t>
         </r>
       </text>
     </comment>
@@ -252,16 +254,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Thomas Ingeman-Nielsen:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Thomas Ingeman-Nielsen:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A meaningful textual description of the feature. Could include information on what measurements or observations were obtained, main results, etc.
 Use ALT+ENTER to make a line break inside a cell.</t>
         </r>
       </text>
@@ -286,7 +289,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Mainly used for images, the direction in which the image was taken.</t>
+Mainly used for images: the cardinal direction (N, S, E, W, SE, NW, etc.) in which the image was taken.</t>
         </r>
       </text>
     </comment>
@@ -573,7 +576,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -608,9 +611,6 @@
     <t>Geometry_type</t>
   </si>
   <si>
-    <t>WGS84 Lon/Lat</t>
-  </si>
-  <si>
     <t>WGS 84 / UTM zone 22N</t>
   </si>
   <si>
@@ -642,9 +642,6 @@
   </si>
   <si>
     <t>SRID code</t>
-  </si>
-  <si>
-    <t>Global projection</t>
   </si>
   <si>
     <t>Most of West Greenland covered</t>
@@ -727,6 +724,57 @@
   </si>
   <si>
     <t>Thule / Qaanaaq area</t>
+  </si>
+  <si>
+    <t>WGS84 Longitude/Latitude</t>
+  </si>
+  <si>
+    <t>Global system, geographical coordinates</t>
+  </si>
+  <si>
+    <t>txt_code</t>
+  </si>
+  <si>
+    <t>utm22_gr96</t>
+  </si>
+  <si>
+    <t>geo_wgs84</t>
+  </si>
+  <si>
+    <t>utm18_wgs84</t>
+  </si>
+  <si>
+    <t>utm19_wgs84</t>
+  </si>
+  <si>
+    <t>utm20_wgs84</t>
+  </si>
+  <si>
+    <t>utm21_wgs84</t>
+  </si>
+  <si>
+    <t>utm22_wgs84</t>
+  </si>
+  <si>
+    <t>utm23_wgs84</t>
+  </si>
+  <si>
+    <t>utm24_wgs84</t>
+  </si>
+  <si>
+    <t>utm25_wgs84</t>
+  </si>
+  <si>
+    <t>utm26_wgs84</t>
+  </si>
+  <si>
+    <t>utm27_wgs84</t>
+  </si>
+  <si>
+    <t>utm28_wgs84</t>
+  </si>
+  <si>
+    <t>utm29_wgs84</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1211,7 @@
   <dimension ref="A1:T78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,7 +1221,7 @@
     <col min="3" max="3" width="15.7109375" style="11" customWidth="1"/>
     <col min="4" max="4" width="23.140625" style="11" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" style="11" customWidth="1"/>
+    <col min="6" max="6" width="14" style="11" customWidth="1"/>
     <col min="7" max="8" width="15.85546875" style="11" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" style="11" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" style="12" customWidth="1"/>
@@ -1185,7 +1233,7 @@
   <sheetData>
     <row r="1" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
@@ -1209,7 +1257,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1</v>
@@ -1291,8 +1339,8 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
       <c r="I6" s="3"/>
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
@@ -2478,18 +2526,18 @@
       <c r="T78"/>
     </row>
   </sheetData>
-  <sheetProtection password="CC3D" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0" sort="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0" sort="0"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
-      <formula1>"point"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>"GEOPHYSICAL DATA,FIELD MEASUREMENT,RESOURCE,PHOTO,SAMPLE,OTHER,BOREHOLE,LAB MEASUREMENT"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="The field value must be taken from the list of choices." sqref="I2:I1048576">
       <formula1>"Approximate, GPS (phase), GPS (code), Unknown"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+      <formula1>"point,line,polygon"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
       <formula1>COUNTIF($B:$B,B1)&lt;2</formula1>
     </dataValidation>
   </dataValidations>
@@ -2513,34 +2561,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D23"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>22</v>
-      </c>
       <c r="C1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2548,13 +2600,16 @@
         <v>3182</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2562,13 +2617,16 @@
         <v>4326</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2576,11 +2634,14 @@
         <v>32618</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2588,13 +2649,16 @@
         <v>32619</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2602,11 +2666,14 @@
         <v>32620</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2614,13 +2681,16 @@
         <v>32621</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2628,13 +2698,16 @@
         <v>32622</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2642,13 +2715,16 @@
         <v>32623</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2656,13 +2732,16 @@
         <v>32624</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2670,13 +2749,16 @@
         <v>32625</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2684,13 +2766,16 @@
         <v>32626</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2698,13 +2783,16 @@
         <v>32627</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2712,13 +2800,16 @@
         <v>32628</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2726,74 +2817,84 @@
         <v>32629</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-    </row>
-    <row r="23" spans="1:4" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="23" spans="1:5" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
     </row>
   </sheetData>
   <sortState ref="A2:D24">
     <sortCondition ref="B2:B24"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A23:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2804,7 +2905,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,13 +2919,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="2"/>
       <c r="E1" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -2832,89 +2933,71 @@
       <c r="I1" s="7"/>
       <c r="J1" s="2"/>
       <c r="K1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>16</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="7"/>
       <c r="J2" s="2"/>
       <c r="K2" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
       <c r="I3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K3" s="10">
-        <f>A3+B3/60+C3/3600</f>
+        <f>IF(A3&gt;=0,A3+B3/60+C3/3600,A3-B3/60-C3/3600)</f>
         <v>0</v>
       </c>
       <c r="L3" s="10">
-        <f>E3+F3/60+G3/3600</f>
+        <f>IF(E3&gt;=0,E3+F3/60+G3/3600,E3-F3/60-G3/3600)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I4" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" s="10">
-        <f t="shared" ref="K4:K23" si="0">A4+B4/60+C4/3600</f>
+        <f t="shared" ref="K4:K23" si="0">IF(A4&gt;=0,A4+B4/60+C4/3600,A4-B4/60-C4/3600)</f>
         <v>0</v>
       </c>
       <c r="L4" s="10">
-        <f t="shared" ref="L4:L23" si="1">E4+F4/60+G4/3600</f>
+        <f t="shared" ref="L4:L23" si="1">IF(E4&gt;=0,E4+F4/60+G4/3600,E4-F4/60-G4/3600)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I5" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" si="0"/>
@@ -2927,7 +3010,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" s="10">
         <f t="shared" si="0"/>
@@ -2940,7 +3023,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I7" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K7" s="10">
         <f t="shared" si="0"/>
@@ -2953,7 +3036,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I8" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K8" s="10">
         <f t="shared" si="0"/>
@@ -2966,7 +3049,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I9" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9" s="10">
         <f t="shared" si="0"/>
@@ -2979,7 +3062,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I10" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K10" s="10">
         <f t="shared" si="0"/>
@@ -2992,7 +3075,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I11" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K11" s="10">
         <f t="shared" si="0"/>
@@ -3005,7 +3088,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I12" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K12" s="10">
         <f t="shared" si="0"/>
@@ -3018,7 +3101,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I13" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K13" s="10">
         <f t="shared" si="0"/>
@@ -3031,7 +3114,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I14" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K14" s="10">
         <f t="shared" si="0"/>
@@ -3044,7 +3127,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I15" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K15" s="10">
         <f t="shared" si="0"/>
@@ -3057,7 +3140,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I16" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K16" s="10">
         <f t="shared" si="0"/>
@@ -3070,7 +3153,7 @@
     </row>
     <row r="17" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I17" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K17" s="10">
         <f t="shared" si="0"/>
@@ -3083,7 +3166,7 @@
     </row>
     <row r="18" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I18" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K18" s="10">
         <f t="shared" si="0"/>
@@ -3096,7 +3179,7 @@
     </row>
     <row r="19" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I19" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K19" s="10">
         <f t="shared" si="0"/>
@@ -3109,7 +3192,7 @@
     </row>
     <row r="20" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I20" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K20" s="10">
         <f t="shared" si="0"/>
@@ -3122,7 +3205,7 @@
     </row>
     <row r="21" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I21" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K21" s="10">
         <f t="shared" si="0"/>
@@ -3135,7 +3218,7 @@
     </row>
     <row r="22" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I22" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K22" s="10">
         <f t="shared" si="0"/>
@@ -3148,7 +3231,7 @@
     </row>
     <row r="23" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I23" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K23" s="10">
         <f t="shared" si="0"/>
@@ -3191,7 +3274,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
@@ -3215,7 +3298,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1</v>
@@ -3238,13 +3321,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3">
         <v>32622</v>
@@ -3256,13 +3339,13 @@
         <v>7427269.1699999999</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J2" s="4">
         <v>41336</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -3275,13 +3358,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F3" s="3">
         <v>4326</v>
@@ -3293,13 +3376,13 @@
         <v>66.940393869999994</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J3" s="4">
         <v>41336</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>

</xml_diff>